<commit_message>
Added and Updated Czech Test Data
</commit_message>
<xml_diff>
--- a/Test Data/Gallery_Accessories.xlsx
+++ b/Test Data/Gallery_Accessories.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5792BC1-265E-44E6-91CD-B5F7AABC7DD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4721EDAB-ACFE-4C8C-BB01-8ED279560D9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="3" r:id="rId1"/>
     <sheet name="Belgium" sheetId="6" r:id="rId2"/>
+    <sheet name="Czech" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
   <si>
     <t>Wg</t>
   </si>
@@ -106,6 +107,12 @@
   </si>
   <si>
     <t>NGC-3478/T2262</t>
+  </si>
+  <si>
+    <t>Czech Market</t>
+  </si>
+  <si>
+    <t>NGC-3477/T1731</t>
   </si>
 </sst>
 </file>
@@ -671,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FB1E1A-05DD-49D0-9147-9D7D528C068A}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -807,4 +814,146 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AFD9C7-46B0-4D85-BE0F-FC93F3180CAE}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test data for markets test cases
</commit_message>
<xml_diff>
--- a/Test Data/Gallery_Accessories.xlsx
+++ b/Test Data/Gallery_Accessories.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4721EDAB-ACFE-4C8C-BB01-8ED279560D9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11EB7F1-DA29-4BAB-ACE3-4F00DD94CD83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="3" r:id="rId1"/>
     <sheet name="Belgium" sheetId="6" r:id="rId2"/>
     <sheet name="Czech" sheetId="7" r:id="rId3"/>
+    <sheet name="Swiss" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="28">
   <si>
     <t>Wg</t>
   </si>
@@ -113,6 +114,12 @@
   </si>
   <si>
     <t>NGC-3477/T1731</t>
+  </si>
+  <si>
+    <t>Switzerland Market</t>
+  </si>
+  <si>
+    <t>NGC-3476/T2343/T2641</t>
   </si>
 </sst>
 </file>
@@ -820,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AFD9C7-46B0-4D85-BE0F-FC93F3180CAE}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,4 +963,146 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8520461E-9FE5-4E84-ABF0-175527E2C253}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>